<commit_message>
updating caltrain and amtrak
</commit_message>
<xml_diff>
--- a/Alternatives/Alternatvie5_01_RailOnly/AmtrakService.xlsx
+++ b/Alternatives/Alternatvie5_01_RailOnly/AmtrakService.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="1280" windowWidth="22240" windowHeight="15200" tabRatio="500"/>
+    <workbookView xWindow="960" yWindow="0" windowWidth="25280" windowHeight="16000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="NO CHANGE" sheetId="1" r:id="rId1"/>
+    <sheet name="ALTERNATIVE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
   <si>
     <t>EA</t>
   </si>
@@ -62,6 +63,18 @@
   <si>
     <t>YEAR 2035</t>
   </si>
+  <si>
+    <t>TT-Fairfield/Vacaville</t>
+  </si>
+  <si>
+    <t>Coliseum - Fairfield/Vacaville</t>
+  </si>
+  <si>
+    <t>No change</t>
+  </si>
+  <si>
+    <t>difference</t>
+  </si>
 </sst>
 </file>
 
@@ -100,12 +113,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,7 +136,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -133,8 +152,48 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -145,8 +204,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -154,6 +222,26 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -161,6 +249,26 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -490,65 +598,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="15.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="B2" s="3" t="s">
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="B3" s="3" t="s">
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2">
+        <f>SUM(C4:C8)</f>
+        <v>1.65</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="2">
+        <f>SUM(E4:E8)</f>
+        <v>0.4</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="2">
+        <f>SUM(G4:G8)</f>
+        <v>1.45</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3" t="s">
+      <c r="I3" s="2">
+        <f>SUM(I4:I8)</f>
+        <v>0.8</v>
+      </c>
+      <c r="J3" s="1">
+        <f>C3+E3+G3+I3</f>
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1">
@@ -563,97 +702,821 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J14" si="0">C4+E4+G4+I4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>120</v>
       </c>
       <c r="C5" s="1">
-        <v>300</v>
+        <f>60/B5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>300</v>
+      </c>
+      <c r="E5" s="1">
+        <f>60/D5</f>
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>120</v>
+      </c>
+      <c r="G5" s="1">
+        <f>60/F5</f>
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>300</v>
+      </c>
+      <c r="I5" s="1">
+        <f>60/H5</f>
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>300</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:E8" si="1">60/B6</f>
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>300</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" ref="G6:G7" si="2">60/F6</f>
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>150</v>
+      </c>
+      <c r="I6" s="1">
+        <f>60/H6</f>
+        <v>0.4</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>80</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>80</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="H7" s="1">
+        <v>300</v>
+      </c>
+      <c r="I7" s="1">
+        <f>60/H7</f>
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>300</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>300</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <f>SUM(C10:C14)</f>
+        <v>1.75</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2">
+        <f>SUM(E10:E14)</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="2">
+        <f>SUM(G10:G14)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="2">
+        <f>SUM(I10:I14)</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>80</v>
+      </c>
+      <c r="C11" s="1">
+        <f>60/B11</f>
+        <v>0.75</v>
+      </c>
+      <c r="D11" s="1">
+        <v>120</v>
+      </c>
+      <c r="E11" s="1">
+        <f>60/D11</f>
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>300</v>
+      </c>
+      <c r="G11" s="1">
+        <f>60/F11</f>
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>300</v>
+      </c>
+      <c r="I11" s="1">
+        <f>60/H11</f>
+        <v>0.2</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>120</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" ref="C12:C13" si="3">60/B12</f>
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>300</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" ref="E12" si="4">60/D12</f>
+        <v>0.2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>300</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" ref="G12:G13" si="5">60/F12</f>
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>120</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>300</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" ref="E13" si="6">60/D13</f>
+        <v>0.2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>300</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>120</v>
+      </c>
+      <c r="I13" s="1">
+        <f>60/H13</f>
+        <v>0.5</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>300</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" ref="G14" si="7">60/F14</f>
+        <v>0.2</v>
+      </c>
+      <c r="H14" s="1">
+        <v>300</v>
+      </c>
+      <c r="I14" s="1">
+        <f>60/H14</f>
+        <v>0.2</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="6"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2">
+        <f>SUM(C4:C8)</f>
+        <v>0.9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2">
+        <f>SUM(E4:E8)</f>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <f>SUM(G4:G8)</f>
+        <v>0.4</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2">
+        <f>SUM(I4:I8)</f>
+        <v>1.45</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2">
+        <f>SUM(K4:K8)</f>
+        <v>0.8</v>
+      </c>
+      <c r="L3" s="2">
+        <f>E3+G3+I3+C3+K3</f>
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="M3" s="5">
+        <v>4.3</v>
+      </c>
+      <c r="N3" s="1">
+        <f>L3-M3</f>
+        <v>0.35000000000000053</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" ref="L4:L14" si="0">E4+G4+I4+C4+K4</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <f>L4-M4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>300</v>
+      </c>
+      <c r="C5" s="4">
+        <f>60/B5</f>
+        <v>0.2</v>
       </c>
       <c r="D5" s="1">
         <v>120</v>
       </c>
       <c r="E5" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
+        <f>60/D5</f>
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>300</v>
+      </c>
+      <c r="G5" s="1">
+        <f>60/F5</f>
+        <v>0.2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>120</v>
+      </c>
+      <c r="I5" s="1">
+        <f>60/H5</f>
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>300</v>
+      </c>
+      <c r="K5" s="1">
+        <f>60/J5</f>
+        <v>0.2</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="M5" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="N5" s="1">
+        <f>L5-M5</f>
+        <v>0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <v>300</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
+      <c r="B6" s="4">
+        <v>300</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" ref="C6:C7" si="1">60/B6</f>
+        <v>0.2</v>
       </c>
       <c r="D6" s="1">
         <v>300</v>
       </c>
       <c r="E6" s="1">
+        <f t="shared" ref="E6:G8" si="2">60/D6</f>
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>300</v>
+      </c>
+      <c r="I6" s="1">
+        <f>60/H6</f>
+        <v>0.2</v>
+      </c>
+      <c r="J6" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
+      <c r="K6" s="1">
+        <f>60/J6</f>
+        <v>0.4</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="N6" s="1">
+        <f>L6-M6</f>
+        <v>0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
+        <v>120</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>300</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
         <v>80</v>
       </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>80</v>
-      </c>
-      <c r="E7" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
+      <c r="I7" s="1">
+        <f>60/H7</f>
+        <v>0.75</v>
+      </c>
+      <c r="J7" s="1">
+        <v>300</v>
+      </c>
+      <c r="K7" s="1">
+        <f>60/J7</f>
+        <v>0.2</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="0"/>
+        <v>1.65</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="N7" s="1">
+        <f>L7-M7</f>
+        <v>-5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1">
-        <v>300</v>
-      </c>
-      <c r="C8" s="1">
-        <v>300</v>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="3" t="s">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>300</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="N8" s="1">
+        <f>L8-M8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2">
+        <f>SUM(C10:C14)</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="2">
+        <f>SUM(E10:E14)</f>
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="G9" s="2">
+        <f>SUM(G10:G14)</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="I9" s="2">
+        <f>SUM(I10:I14)</f>
+        <v>0.8</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="2">
+        <f>SUM(K10:K14)</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="0"/>
+        <v>4.7</v>
+      </c>
+      <c r="M9" s="5">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="N9" s="1">
+        <f>L9-M9</f>
+        <v>0.35000000000000053</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
         <v>0</v>
       </c>
       <c r="D10" s="1">
@@ -662,78 +1525,245 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="3" t="s">
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <f>L10-M10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="1">
-        <v>80</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B11" s="4">
         <v>120</v>
       </c>
+      <c r="C11" s="4">
+        <f>60/B11</f>
+        <v>0.5</v>
+      </c>
       <c r="D11" s="1">
-        <v>300</v>
+        <v>120</v>
       </c>
       <c r="E11" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="3" t="s">
+        <f>60/D11</f>
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>300</v>
+      </c>
+      <c r="G11" s="1">
+        <f>60/F11</f>
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>300</v>
+      </c>
+      <c r="I11" s="1">
+        <f>60/H11</f>
+        <v>0.2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>300</v>
+      </c>
+      <c r="K11" s="1">
+        <f>60/J11</f>
+        <v>0.2</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="M11" s="5">
+        <v>1.65</v>
+      </c>
+      <c r="N11" s="1">
+        <f>L11-M11</f>
+        <v>-5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="4">
+        <v>300</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" ref="C12:C13" si="3">60/B12</f>
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="1">
         <v>120</v>
       </c>
-      <c r="C12" s="1">
-        <v>300</v>
-      </c>
-      <c r="D12" s="1">
-        <v>300</v>
-      </c>
       <c r="E12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3" t="s">
+        <f t="shared" ref="E12:E13" si="4">60/D12</f>
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>300</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" ref="G12:G13" si="5">60/F12</f>
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="1">
+        <v>300</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" ref="I12:I14" si="6">60/H12</f>
+        <v>0.2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="N12" s="1">
+        <f>L12-M12</f>
+        <v>0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="4">
+        <v>300</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="1">
         <v>120</v>
       </c>
-      <c r="C13" s="1">
-        <v>300</v>
-      </c>
-      <c r="D13" s="1">
-        <v>300</v>
-      </c>
       <c r="E13" s="1">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>300</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>300</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="6"/>
+        <v>0.2</v>
+      </c>
+      <c r="J13" s="1">
         <v>120</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
+      <c r="K13" s="1">
+        <f>60/J13</f>
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="M13" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="N13" s="1">
+        <f>L13-M13</f>
+        <v>0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>300</v>
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>300</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="6"/>
+        <v>0.2</v>
+      </c>
+      <c r="J14" s="1">
+        <v>300</v>
+      </c>
+      <c r="K14" s="1">
+        <f>60/J14</f>
+        <v>0.2</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="N14" s="1">
+        <f>L14-M14</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+  <mergeCells count="7">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>